<commit_message>
Adding support for H2 version 2.x
</commit_message>
<xml_diff>
--- a/hotrod-project/docs/research/live-sql/functions.xlsx
+++ b/hotrod-project/docs/research/live-sql/functions.xlsx
@@ -818,11 +818,11 @@
   </sheetPr>
   <dimension ref="A1:I105"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D67" activeCellId="0" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.47"/>
@@ -2021,7 +2021,7 @@
         <v>116</v>
       </c>
       <c r="D66" s="13" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>117</v>
@@ -2455,7 +2455,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.67"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="2" style="1" width="11.52"/>

</xml_diff>